<commit_message>
aggiunta intefaccia per la funzione utilità; refactoring
</commit_message>
<xml_diff>
--- a/Grid Planner/lib/SARLib/Toolbox/analisi aggiornamento confidenza.xlsx
+++ b/Grid Planner/lib/SARLib/Toolbox/analisi aggiornamento confidenza.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="upd_confidence_RND_grid" localSheetId="0">Data!$B$66:$F$75</definedName>
     <definedName name="update_confidence_false_target" localSheetId="0">Data!$B$9:$F$18</definedName>
     <definedName name="update_confidence_true_target" localSheetId="0">Data!#REF!</definedName>
     <definedName name="update_confidence_true_target_1" localSheetId="0">Data!$B$43:$F$52</definedName>
@@ -52,11 +53,22 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="3" name="upd-confidence RND_grid" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\filip\Dropbox\Unimi\pianificazione\Grid Planner\lib\SARLib\Toolbox\upd-confidence RND_grid.txt" semicolon="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Sensed True Target</t>
   </si>
@@ -84,12 +96,18 @@
   <si>
     <t>Sensed False Target</t>
   </si>
+  <si>
+    <t>UPDATING CONFIDENCE</t>
+  </si>
+  <si>
+    <t>POINT: (2,5)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,13 +123,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -132,15 +174,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2480,6 +2528,1844 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1823240767"/>
+        <c:crosses val="autoZero"/>
+      </c:serAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="90"/>
+      <c:rotY val="0"/>
+      <c:rAngAx val="0"/>
+      <c:perspective val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:surfaceChart>
+        <c:wireframe val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$B$65</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent2">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data!$A$66:$A$75</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$B$66:$B$75</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.30299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.33100000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.371</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.52400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.42799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.33100000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.30299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F94D-4391-9846-2F30DA28F78E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$C$65</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent4">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data!$A$66:$A$75</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$C$66:$C$75</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.33100000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.371</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.42799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.52400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.84499999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.42799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.371</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.30299999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F94D-4391-9846-2F30DA28F78E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$D$65</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent6">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data!$A$66:$A$75</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$D$66:$D$75</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.371</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.42799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.52400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.84499999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.8999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.84499999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.52400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.42799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.371</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.33100000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F94D-4391-9846-2F30DA28F78E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$E$65</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data!$A$66:$A$75</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$E$66:$E$75</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.33100000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.371</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.42799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.52400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.52400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.42799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.371</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.33100000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.30299999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F94D-4391-9846-2F30DA28F78E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$F$65</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data!$A$66:$A$75</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$F$66:$F$75</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.30299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.33100000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.371</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.52400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.33100000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-F94D-4391-9846-2F30DA28F78E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:bandFmts>
+          <c:bandFmt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent2">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent4">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent6">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="7"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="8"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="9"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="80000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="80000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="80000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="80000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="80000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="10"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="80000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="80000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="80000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="80000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="80000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="11"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="80000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="80000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="80000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="80000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="80000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="12"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="13"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="14"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:bandFmt>
+        </c:bandFmts>
+        <c:axId val="1294948527"/>
+        <c:axId val="1291469327"/>
+        <c:axId val="1338459071"/>
+      </c:surfaceChart>
+      <c:catAx>
+        <c:axId val="1294948527"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1291469327"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1291469327"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="none"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1294948527"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="1338459071"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1291469327"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
       <c:spPr>
@@ -2632,14 +4518,54 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>438912</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93519827-335D-4B2B-ACDB-C25A3042B501}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="upd-confidence RND_grid" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="update confidence_true target_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="update confidence_false target" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -2940,10 +4866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M88" sqref="M88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3024,7 +4950,7 @@
       <c r="E9">
         <v>0.84499999999999997</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>5.8999999999999997E-2</v>
       </c>
     </row>
@@ -3461,7 +5387,7 @@
       <c r="A52">
         <v>0</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="3">
         <v>0.94099999999999995</v>
       </c>
       <c r="C52">
@@ -3474,6 +5400,261 @@
         <v>0</v>
       </c>
       <c r="F52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <f>B65+1</f>
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <f>C65+1</f>
+        <v>2</v>
+      </c>
+      <c r="E65">
+        <f>D65+1</f>
+        <v>3</v>
+      </c>
+      <c r="F65">
+        <f>E65+1</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <f t="shared" ref="A66:A73" si="2">A67+1</f>
+        <v>9</v>
+      </c>
+      <c r="B66">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="C66">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="D66">
+        <v>0.371</v>
+      </c>
+      <c r="E66">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="F66">
+        <v>0.30299999999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="B67">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="C67">
+        <v>0.371</v>
+      </c>
+      <c r="D67">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="E67">
+        <v>0.371</v>
+      </c>
+      <c r="F67">
+        <v>0.33100000000000002</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="B68">
+        <v>0.371</v>
+      </c>
+      <c r="C68">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="D68">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="E68">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="F68">
+        <v>0.371</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="D69">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="E69">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="B70">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="C70">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="D70">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>0.52400000000000002</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="B71">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="E71">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="D72">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="E72">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="B73">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="C73">
+        <v>0.371</v>
+      </c>
+      <c r="D73">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="E73">
+        <v>0.371</v>
+      </c>
+      <c r="F73">
+        <v>0.33100000000000002</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <f>A75+1</f>
+        <v>1</v>
+      </c>
+      <c r="B74">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0.371</v>
+      </c>
+      <c r="E74">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>0</v>
+      </c>
+      <c r="B75">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C75">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="D75">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="E75">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="F75">
         <v>0</v>
       </c>
     </row>

</xml_diff>